<commit_message>
variables and model defined
</commit_message>
<xml_diff>
--- a/Gen_S_Variables.xlsx
+++ b/Gen_S_Variables.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcsoliman/FinTech/Project_01/Project-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcsoliman/FinTech/Project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A458084C-FB85-0049-952D-11B0D8073C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CC9A2C-EC9F-F648-A7D6-981391F959B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{668433BF-F93D-4941-9368-88DF3B5A1A25}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="29060" windowHeight="18700" activeTab="1" xr2:uid="{668433BF-F93D-4941-9368-88DF3B5A1A25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="Model" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Sources</t>
   </si>
@@ -289,13 +291,73 @@
   </si>
   <si>
     <t>Policy - housing programs</t>
+  </si>
+  <si>
+    <t>RISK OBLIVIOUS</t>
+  </si>
+  <si>
+    <t>RISK PRONE</t>
+  </si>
+  <si>
+    <t>RISK AVERSE</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>CRIME RATE</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>PEOPLE</t>
+  </si>
+  <si>
+    <t>PLACE</t>
+  </si>
+  <si>
+    <t>INCOME</t>
+  </si>
+  <si>
+    <t>POLICY</t>
+  </si>
+  <si>
+    <t>OPPORTUNITY ZONES</t>
+  </si>
+  <si>
+    <t>PUBLIC TRANSPORT/PARK SPENDING/PUBLIC HOUSING</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>data source</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>tabula-py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +391,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -373,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -387,26 +456,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -424,6 +502,290 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>145673</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>107068</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>974713</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>404068</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A830AA4-6D37-124A-839E-DE258B55E850}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2902320" y="510480"/>
+            <a:ext cx="3623040" cy="297000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A830AA4-6D37-124A-839E-DE258B55E850}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2893680" y="501480"/>
+              <a:ext cx="3640680" cy="314640"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>119033</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>93167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1138873</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>466127</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B1232A-6069-CC48-A223-B09A6D70314E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2875680" y="1019520"/>
+            <a:ext cx="3813840" cy="372960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B1232A-6069-CC48-A223-B09A6D70314E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2866680" y="1010520"/>
+              <a:ext cx="3831480" cy="390600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>197873</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>39306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1099993</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>430626</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24304CCD-C4E6-404C-800A-0029478F902C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2954520" y="1488600"/>
+            <a:ext cx="3696120" cy="391320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24304CCD-C4E6-404C-800A-0029478F902C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2945520" y="1479960"/>
+              <a:ext cx="3713760" cy="408960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-10-12T16:56:02.557"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 48 24575,'4'-6'0,"15"2"0,-5 4 0,19 0 0,-16 0 0,8 0 0,-6 0 0,1-6 0,3 5 0,-3-5 0,4 6 0,4 0 0,-7 0 0,7 0 0,-11-3 0,1 3 0,-2-3 0,0 3 0,3-3 0,-3 2 0,0-2 0,-1 3 0,-3-2 0,3 1 0,-2-2 0,2 3 0,0 0 0,-2-2 0,2 1 0,-3-2 0,0 3 0,0 0 0,3 0 0,-2 0 0,2 0 0,0 0 0,-2 0 0,2 0 0,-3 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,3 0 0,-2 0 0,2 0 0,0 0 0,-2 0 0,2 0 0,0 0 0,-2 0 0,5 3 0,-5-2 0,6 2 0,-3 0 0,3-3 0,-3 6 0,3-5 0,-3 4 0,3-1 0,-3-1 0,3 3 0,-3-5 0,12 4 0,-6-4 0,6 5 0,-9-5 0,0 4 0,5-4 0,-4 5 0,0-3 0,-1 1 0,-3 1 0,3-4 0,1 5 0,-1-6 0,1 6 0,-1-5 0,1 5 0,-1-6 0,0 6 0,1-2 0,-4 2 0,2-3 0,-1 3 0,-1-3 0,2 1 0,-5 1 0,5-4 0,-2 4 0,1-1 0,1-1 0,-5 2 0,5-1 0,-2-1 0,4 3 0,-1-2 0,-3 2 0,7-3 0,-6 3 0,6-3 0,-4 1 0,1 2 0,-1-3 0,1 4 0,-1-1 0,1-2 0,-1 2 0,1-3 0,-1 4 0,-3-4 0,3 3 0,-3-5 0,3 5 0,-3-6 0,12 6 0,-14-3 0,14 1 0,-12 1 0,3-4 0,0 5 0,1-2 0,-1-1 0,1 3 0,3-5 0,-2 1 0,6 2 0,-3-4 0,0 3 0,4 1 0,-4-4 0,4 3 0,-3 0 0,-2-2 0,0 2 0,-2 0 0,2-2 0,0 1 0,-2-2 0,2 0 0,1 0 0,-4 3 0,7-2 0,-6 2 0,6-3 0,-2 0 0,3 0 0,0 0 0,0 3 0,1-2 0,3 2 0,-3-3 0,4 0 0,-5 0 0,0 0 0,-3 0 0,2 0 0,-3 0 0,0 0 0,4 0 0,-8 0 0,7 0 0,-6 0 0,2 0 0,-4 0 0,5 0 0,-4 0 0,7 0 0,-2 0 0,-1 0 0,3 0 0,-2 0 0,-1 0 0,3 0 0,-6 0 0,6 0 0,-7 0 0,4 0 0,-5 0 0,1 0 0,-4 0 0,2 0 0,-2 0 0,1 0 0,1 0 0,-5 3 0,5-3 0,-2 6 0,4-6 0,-4 6 0,3-5 0,-3 4 0,7-4 0,-3 2 0,4 0 0,-1-3 0,1 3 0,1-3 0,2 0 0,-3 3 0,4-2 0,13 5 0,-13-5 0,11 2 0,-14 0 0,-1-2 0,3 2 0,-6 0 0,2-2 0,-4 5 0,1-3 0,-1 1 0,1-1 0,-1 0 0,1-3 0,-4 6 0,2-3 0,-2 1 0,4 1 0,-1-4 0,5 5 0,-4-5 0,4 5 0,-5-5 0,4 5 0,-2-6 0,6 7 0,-7-6 0,8 5 0,-4-2 0,4 0 0,-3 2 0,2-2 0,-3-1 0,5 3 0,-1-2 0,0 3 0,0 0 0,5-3 0,-3 3 0,2-7 0,1 7 0,-4-3 0,8 0 0,-3 3 0,0-7 0,3 4 0,-8-1 0,4-2 0,-5 5 0,0-5 0,1 5 0,-1-5 0,-4 5 0,4-5 0,-4 5 0,4-6 0,0 7 0,1-3 0,-1-1 0,0 4 0,9 0 0,-7-3 0,7 5 0,-13-5 0,4 3 0,-8-1 0,7 1 0,-6 0 0,6 0 0,-3 0 0,1-1 0,2 1 0,-3 0 0,4 0 0,-3 0 0,2 0 0,-7 0 0,8-4 0,-8 3 0,7-2 0,-6 0 0,6 2 0,-2-5 0,3 5 0,0-5 0,0 2 0,0 0 0,1-2 0,-1 2 0,-4-3 0,4 3 0,-4-2 0,0 2 0,3-3 0,-2 3 0,-1-2 0,3 2 0,-6 0 0,6-2 0,-3 2 0,1-3 0,-2 0 0,0 0 0,-2 0 0,15 0 0,-10 0 0,11 0 0,-9 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,-4 0 0,3 0 0,-6 0 0,-1 0 0,-2 0 0,-1 0 0,-1 0 0,2 0 0,-5 0 0,5 0 0,-2 0 0,0 0 0,3 0 0,-3 0 0,4 0 0,-1 0 0,0 0 0,5 0 0,-4 0 0,4 0 0,-5 0 0,1 0 0,-1 0 0,0 0 0,5 0 0,-7 0 0,5 0 0,-6 2 0,4-1 0,-1 2 0,-3-3 0,3 3 0,-7-2 0,7 1 0,-6-2 0,2 3 0,-3-2 0,3 1 0,-2-2 0,2 0 0,-3 3 0,0-2 0,3 1 0,1-2 0,3 3 0,1-2 0,-1 2 0,4-3 0,-2 0 0,6 0 0,-3 0 0,0 0 0,12 0 0,-9 0 0,6 0 0,-10 0 0,-3 0 0,-4 0 0,2 0 0,-5 0 0,5 0 0,-5 2 0,2-1 0,1 2 0,-7-3 0,6 0 0,-6 0 0,3 0 0,-1 0 0,1 0 0,0 0 0,-3 0 0,2 0 0,-2 0 0,3 0 0,0 0 0,-3 0 0,2 0 0,-2 0 0,3 0 0,-1 0 0,1 0 0,0 0 0,3 0 0,-2 0 0,2 0 0,-3 0 0,0 0 0,3 0 0,1 0 0,0 0 0,2 0 0,-5 2 0,2-1 0,6 2 0,-7-3 0,6 2 0,-8-1 0,0 1 0,-3-2 0,2 0 0,-2 0 0,3 3 0,-3-2 0,2 1 0,-2-2 0,2 0 0,1 0 0,-3 0 0,2 3 0,-2-2 0,3 1 0,0-2 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,3 0 0,-2 0 0,2 0 0,0 0 0,1 0 0,0 0 0,3 0 0,-7 0 0,7 0 0,-3 0 0,4 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-3 0,-1 3 0,1-3 0,-4 0 0,2 2 0,-2-1 0,0-1 0,3 2 0,-3-4 0,3 4 0,1-2 0,-1 3 0,1 0 0,-1 0 0,4-3 0,-2 2 0,2-2 0,0 3 0,10-3 0,-2 2 0,2-2 0,-10 3 0,0 0 0,-2 0 0,2 0 0,-7-2 0,3 1 0,-3-2 0,0 3 0,-1 0 0,-3 0 0,0 0 0,-1 0 0,-2 0 0,2 0 0,-2 0 0,3 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-3 0 0,2 0 0,-2 0 0,0 0 0,-1 0 0,1 0 0,-3 0 0,2 0 0,-3 0 0,0 0 0,1 0 0,-1 0 0,-2 3 0,1-3 0,-3 2 0,1-2 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-10-12T16:56:43.638"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1035 24575,'22'0'0,"8"0"0,-8 0 0,30 0 0,-26 0 0,49 0 0,-48 0 0,55 0 0,-36-4 0,34-1 0,-17-7 0,10 1 0,-10-1 0,-5 3 0,1 0 0,-8 1 0,10-1 0,13 0 0,-24 1 0,21-2 0,-19-2 0,12 2 0,-7-3 0,2 4 0,4-4 0,-13 4 0,15-8 0,-20 8 0,6-7 0,22-3 0,-29 6 0,21-9 0,-25 10 0,27-6 0,-22 5 0,38-10 0,-33 13 0,24-13 0,-13 14 0,-9-4 0,7 5 0,4-10 0,-13 7 0,33-12 0,-27 14 0,20-9 0,-3 4 0,-3-5 0,5 5 0,6-5 0,-4 5 0,11-2 0,-11-2 0,4 3 0,-6 1 0,7-4 0,-5 7 0,11-3 0,-5-1 0,0 5 0,-13-4 0,2 5 0,5-1 0,1 1 0,10-1 0,-19 5 0,4-3 0,2 2 0,8-4 0,0 5 0,6-4 0,-13 8 0,6-8 0,-23 8 0,25-8 0,-22 8 0,27-4 0,-14 1 0,0 3 0,0-7 0,7 7 0,-6-4 0,6 1 0,-1 3 0,2-8 0,7 8-702,6-8 702,3 3 0,-47 1 0,1 0 0,0-1 0,0 1 0,3 0 0,0-1 0,-2 1 0,0 0 0,2-1 0,0 1 0,-3-3 0,0 0 0,0 3 0,-1-1 0,1-2 0,0 0 0,-1 0 0,1 1 0,0 1 0,0 0 0,45-9 0,-1 5 0,-31 4-87,32-3 87,-51 4 0,44 0 0,-26 1 0,-9 4 0,14 0 0,-29 0 0,14 0 698,-11 0-698,-1 0 91,-4 0-91,-6 0 0,0 0 0,-5 0 0,0 0 0,-3 0 0,2 0 0,-7 0 0,20 0 0,-16 3 0,15 1 0,-14 3 0,12 0 0,-6-3 0,11 0 0,-8-1 0,4 2 0,0-1 0,5 3 0,-3-3 0,3 1 0,-5 1 0,1-1 0,-6-1 0,4 3 0,-7-7 0,7 7 0,-8-6 0,19 6 0,-16-6 0,32 3 0,-22-4 0,14 0 0,-8 0 0,2 0 0,1 0 0,9 0 0,-9 0 0,4 0 0,-6 0 0,12 0 0,-18 0 0,15 0 0,-6 0 0,5 0 0,-4-3 0,-1-1 0,-12-4 0,4 0 0,-1 3 0,-9-1 0,-2 2 0,-7 0 0,2-2 0,2 2 0,-4-3 0,7 3 0,-11 2 0,6-2 0,-7 4 0,8-7 0,-4 6 0,1-2 0,2 0 0,-3 2 0,0-2 0,0 0 0,-1 3 0,-2-3 0,2 0 0,-4 2 0,-3-2 0,0 3 0,-5 0 0,-2 0 0,3 0 0,-6 0 0,2 0 0,-3 0 0,0 0 0,-2 0 0,-1 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-10-12T16:56:59.944"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1087 24575,'21'0'0,"1"0"0,21 0 0,-2 0 0,25 0 0,4 0 0,13 0 0,7 0-483,-20 0 0,0 0 483,14 0 0,-5 0 0,0 0 0,5 0 0,-20 0 0,1 0 0,-15 0 0,0 0-200,6 0 0,-2 0 200,31 0 0,9 0 0,-10 0 0,-1 0 0,5 0 0,-12 0 0,12 0 0,-11 0 0,-1 0 0,-3 0 0,-4 0-14,0 0 14,5 0 0,1 0 0,2-4 0,4 3 0,-6-7 0,0 6 0,-17-5 0,13 6 0,2-7 0,-1 3 0,15-5 0,-18 5 0,6-3 0,0 2 0,0-3 945,-20 1-945,14-2 420,-1-3-420,-10 3 15,32-5-15,-40 3 0,24 2 0,-7-3 0,-4 4 0,10-4 0,-4 2 0,6-2 0,0-1 0,0 4 0,6-4 0,-4 0 0,5 4 0,-8-4 0,-5 5 0,4 0 0,-3-1 0,-16 2 0,10-1 0,2 0 0,-14 1 0,37-6 0,-39 5 0,17-5 0,-7 6 0,2-1 0,1 0 0,4 0 0,1 0 0,1 0 0,-11 3 0,7-2 0,-13 3 0,28-4 0,-14 0 0,14-1 0,-19 5 0,6-3 0,2 3 0,-15-3 0,0-2 0,30-1 0,-30 2 0,0 0 0,21 0 0,0-5 0,-7 4 0,5-7 0,-3 6 0,4-2 0,-5 0 0,4 2 0,-20 3 0,18-5 0,-6 6 0,-4-5 0,10 2 0,-25 6 0,27-9 0,-14 7 0,15-4 0,-12 2 0,-15 7 0,30-7 0,-40 3 0,35-4 0,-32 5 0,14-4 0,-3 7 0,-1-6 0,-2 3 0,7-1 0,-3-2 0,-1 6 0,-9-6 0,-3 6 0,0-6 0,9 3 0,-3-4 0,-1 0 0,-1 3 0,-5-2 0,0 3 0,0-4 0,1 1 0,-1-1 0,5 0 0,13-5 0,-14 4 0,28-8 0,-32 8 0,49-7 0,-36 7 0,26-4 0,-28 5 0,1-4 0,-6 3 0,-1-2 0,-5 3 0,0 0 0,-4 4 0,3-3 0,-8 3 0,0 0 0,-2-2 0,-6 5 0,2-2 0,-3 3 0,-1 0 0,1-3 0,-4 2 0,2-2 0,-2 3 0,0 0 0,3 0 0,-6-3 0,5 3 0,2-6 0,1 5 0,2-2 0,-3 0 0,3 2 0,-6-2 0,6 0 0,-7 3 0,0-3 0,-1 3 0,0 0 0,-5 0 0,4 0 0,-5 0 0,0 0 0,0 0 0,-4 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-3 0 0,-1 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -725,16 +1087,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0733045A-A05D-E44F-A3A6-C3C93728035A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="49" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="18.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" style="2" customWidth="1"/>
@@ -765,572 +1127,572 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="C23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="6" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="11" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="11" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="11" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="11" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="11" t="s">
+      <c r="C36" s="5"/>
+      <c r="D36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="5"/>
+      <c r="D37" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="11" t="s">
+      <c r="C38" s="5"/>
+      <c r="D38" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="11" t="s">
+      <c r="C39" s="5"/>
+      <c r="D39" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1346,4 +1708,140 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E153CE1-8D0C-964D-8984-97BBFCBE2BEF}">
+  <dimension ref="A2:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="13" customWidth="1"/>
+    <col min="5" max="7" width="18.33203125" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B65AD8-32CF-FC4D-BE4C-34DA7A886D32}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
column for data link
</commit_message>
<xml_diff>
--- a/Gen_S_Variables.xlsx
+++ b/Gen_S_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcsoliman/FinTech/Project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CC9A2C-EC9F-F648-A7D6-981391F959B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2F2237-D76A-2247-A094-7ABC5F303B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="29060" windowHeight="18700" activeTab="1" xr2:uid="{668433BF-F93D-4941-9368-88DF3B5A1A25}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
   <si>
     <t>Sources</t>
   </si>
@@ -344,20 +344,38 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>data source</t>
-  </si>
-  <si>
     <t>SQL</t>
   </si>
   <si>
     <t>tabula-py</t>
+  </si>
+  <si>
+    <t>Link to data source</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Investment Zone</t>
+  </si>
+  <si>
+    <t>Stable Zone</t>
+  </si>
+  <si>
+    <t>IRS SOI by zip code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -399,8 +417,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,8 +438,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -437,12 +486,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -468,6 +579,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -478,13 +592,70 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -508,19 +679,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>145673</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>174536</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>107068</xdr:rowOff>
+      <xdr:rowOff>164795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>974713</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1003577</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>404068</xdr:rowOff>
+      <xdr:rowOff>461795</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -534,12 +705,12 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="2902320" y="510480"/>
-            <a:ext cx="3623040" cy="297000"/>
+            <a:off x="9309877" y="799795"/>
+            <a:ext cx="3628813" cy="297000"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -573,19 +744,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>119033</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>93167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1138873</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1138874</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>466127</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -604,7 +775,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -638,19 +809,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>197873</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>39306</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1099993</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1099994</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>430626</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
@@ -669,7 +840,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Ink 4">
@@ -1127,7 +1298,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1144,7 +1315,7 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1330,7 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1345,7 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1189,7 +1360,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1204,7 +1375,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1219,7 +1390,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1234,7 +1405,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1251,7 +1422,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1266,7 +1437,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1281,7 +1452,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
@@ -1296,7 +1467,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1311,7 +1482,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
@@ -1326,7 +1497,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="5" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1512,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="5" t="s">
         <v>36</v>
       </c>
@@ -1356,7 +1527,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="5" t="s">
         <v>38</v>
       </c>
@@ -1371,7 +1542,7 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1386,7 +1557,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
@@ -1401,7 +1572,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="5" t="s">
         <v>44</v>
       </c>
@@ -1416,7 +1587,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
@@ -1431,7 +1602,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1446,7 +1617,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="5" t="s">
         <v>50</v>
       </c>
@@ -1461,7 +1632,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
@@ -1474,7 +1645,7 @@
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="5" t="s">
         <v>54</v>
       </c>
@@ -1487,7 +1658,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="5" t="s">
         <v>57</v>
       </c>
@@ -1500,7 +1671,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="5" t="s">
         <v>58</v>
       </c>
@@ -1513,7 +1684,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="5" t="s">
         <v>61</v>
       </c>
@@ -1526,7 +1697,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="5" t="s">
         <v>62</v>
       </c>
@@ -1539,7 +1710,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="5" t="s">
         <v>64</v>
       </c>
@@ -1552,7 +1723,7 @@
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
@@ -1565,7 +1736,7 @@
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="5" t="s">
         <v>68</v>
       </c>
@@ -1578,7 +1749,7 @@
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="5" t="s">
         <v>71</v>
       </c>
@@ -1591,7 +1762,7 @@
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="5" t="s">
         <v>72</v>
       </c>
@@ -1604,7 +1775,7 @@
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="5" t="s">
         <v>76</v>
       </c>
@@ -1617,7 +1788,7 @@
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="5" t="s">
         <v>74</v>
       </c>
@@ -1630,7 +1801,7 @@
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1645,7 +1816,7 @@
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="5" t="s">
         <v>79</v>
       </c>
@@ -1658,7 +1829,7 @@
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="5" t="s">
         <v>80</v>
       </c>
@@ -1671,7 +1842,7 @@
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="5" t="s">
         <v>81</v>
       </c>
@@ -1684,7 +1855,7 @@
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="5" t="s">
         <v>85</v>
       </c>
@@ -1712,125 +1883,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E153CE1-8D0C-964D-8984-97BBFCBE2BEF}">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="13" customWidth="1"/>
-    <col min="5" max="7" width="18.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="18.1640625" style="13" customWidth="1"/>
+    <col min="6" max="8" width="18.33203125" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="C2" s="13" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B4" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="21" t="s">
         <v>101</v>
       </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{8CC1A384-7EA7-704E-92CC-21A6C28B0898}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added links to historical sales data & development data
</commit_message>
<xml_diff>
--- a/Gen_S_Variables.xlsx
+++ b/Gen_S_Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcsoliman/FinTech/Project-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekuo651\Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2F2237-D76A-2247-A094-7ABC5F303B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DCF032-B41C-4EBB-A1F9-E0F5744EBCFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="29060" windowHeight="18700" activeTab="1" xr2:uid="{668433BF-F93D-4941-9368-88DF3B5A1A25}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{668433BF-F93D-4941-9368-88DF3B5A1A25}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t>Sources</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>IRS SOI by zip code</t>
+  </si>
+  <si>
+    <t>Historical Sales Data by Borough</t>
+  </si>
+  <si>
+    <t>NYC OPEN DATA DOB Job Filings</t>
   </si>
 </sst>
 </file>
@@ -582,6 +588,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -591,71 +660,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1262,19 +1268,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="49" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
     <col min="4" max="4" width="32.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="18.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="10.796875" style="2"/>
+    <col min="6" max="6" width="18.796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.796875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1297,8 +1303,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1314,8 +1320,8 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1329,8 +1335,8 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1344,8 +1350,8 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1359,8 +1365,8 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1374,8 +1380,8 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1389,8 +1395,8 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1404,8 +1410,8 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1421,8 +1427,8 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1436,8 +1442,8 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="31"/>
       <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1451,8 +1457,8 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="31"/>
       <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
@@ -1466,8 +1472,8 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1481,8 +1487,8 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
@@ -1496,8 +1502,8 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
       <c r="B15" s="5" t="s">
         <v>35</v>
       </c>
@@ -1511,8 +1517,8 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
       <c r="B16" s="5" t="s">
         <v>36</v>
       </c>
@@ -1526,8 +1532,8 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
         <v>38</v>
       </c>
@@ -1541,8 +1547,8 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="31"/>
       <c r="B18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1556,8 +1562,8 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="31"/>
       <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
@@ -1571,8 +1577,8 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
         <v>44</v>
       </c>
@@ -1586,8 +1592,8 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="31"/>
       <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
@@ -1601,8 +1607,8 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="31"/>
       <c r="B22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1616,8 +1622,8 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="31"/>
       <c r="B23" s="5" t="s">
         <v>50</v>
       </c>
@@ -1631,8 +1637,8 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="31"/>
       <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
@@ -1644,8 +1650,8 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="31"/>
       <c r="B25" s="5" t="s">
         <v>54</v>
       </c>
@@ -1657,8 +1663,8 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="31"/>
       <c r="B26" s="5" t="s">
         <v>57</v>
       </c>
@@ -1670,8 +1676,8 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="31"/>
       <c r="B27" s="5" t="s">
         <v>58</v>
       </c>
@@ -1683,8 +1689,8 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="31"/>
       <c r="B28" s="5" t="s">
         <v>61</v>
       </c>
@@ -1696,8 +1702,8 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="31"/>
       <c r="B29" s="5" t="s">
         <v>62</v>
       </c>
@@ -1709,8 +1715,8 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="31"/>
       <c r="B30" s="5" t="s">
         <v>64</v>
       </c>
@@ -1722,8 +1728,8 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="31"/>
       <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
@@ -1735,8 +1741,8 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="31"/>
       <c r="B32" s="5" t="s">
         <v>68</v>
       </c>
@@ -1748,8 +1754,8 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="31"/>
       <c r="B33" s="5" t="s">
         <v>71</v>
       </c>
@@ -1761,8 +1767,8 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="31"/>
       <c r="B34" s="5" t="s">
         <v>72</v>
       </c>
@@ -1774,8 +1780,8 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="31"/>
       <c r="B35" s="5" t="s">
         <v>76</v>
       </c>
@@ -1787,8 +1793,8 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="31"/>
       <c r="B36" s="5" t="s">
         <v>74</v>
       </c>
@@ -1800,8 +1806,8 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1815,8 +1821,8 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>79</v>
       </c>
@@ -1828,8 +1834,8 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="31"/>
       <c r="B39" s="5" t="s">
         <v>80</v>
       </c>
@@ -1841,8 +1847,8 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="31"/>
       <c r="B40" s="5" t="s">
         <v>81</v>
       </c>
@@ -1854,8 +1860,8 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="31"/>
       <c r="B41" s="5" t="s">
         <v>85</v>
       </c>
@@ -1885,164 +1891,168 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E153CE1-8D0C-964D-8984-97BBFCBE2BEF}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="88" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" style="14" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="13" customWidth="1"/>
-    <col min="4" max="5" width="18.1640625" style="13" customWidth="1"/>
-    <col min="6" max="8" width="18.33203125" style="9" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="8.796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.296875" style="10" customWidth="1"/>
+    <col min="4" max="5" width="18.19921875" style="10" customWidth="1"/>
+    <col min="6" max="8" width="18.296875" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="10.796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="32" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="29" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="27"/>
-    </row>
-    <row r="5" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="27"/>
-    </row>
-    <row r="6" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="E5" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="27"/>
-    </row>
-    <row r="7" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="E6" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2050,9 +2060,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{8CC1A384-7EA7-704E-92CC-21A6C28B0898}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{F0882A68-C0ED-4BF5-9D34-51AAAE00B878}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{B8585A0F-A539-4023-8713-160B010FE4DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2062,7 +2074,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>